<commit_message>
Improved parsing for digikey data and part attributes
Added LEDs, and Tantalum caps

Added junctions.

Added get_manifest() to some EagleFileParts to extract listing of what they contain.

cleanup the version of NVSL.lbr used for testing

Fixes to NVSLLayers.lbr

Additional symbols in Symbols.lbr

Tools for building and manipulating libraries:  buildResolverParts.py and mergeLibrary.py 

Improved part resolver.

Commandline tool to extract a list of file contents:  statEagle.py



git-svn-id: svn+ssh://bbfs-01.calit2.net/grw/Gordon/svn/trunk/Gadgets/Tools/CircuitsByCode@20061 2cf53259-273a-af40-bda6-69d31023b8ec
</commit_message>
<xml_diff>
--- a/Ceramic-Capacitors-0805.xlsx
+++ b/Ceramic-Capacitors-0805.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="download (5).csv" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -4522,7 +4522,7 @@
   <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AH387"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="27080" topLeftCell="AC1"/>
       <selection activeCell="AG2" sqref="AG2"/>
       <selection pane="topRight" activeCell="AF31" sqref="AF31"/>

</xml_diff>